<commit_message>
committing on 13-JUL-20 part 4
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8F12C4-675E-40BB-BD3D-74A206D142D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25380EB-FFB6-47D4-8E40-A8495180E452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -34,11 +34,10 @@
     <sheet name="Payer" sheetId="23" r:id="rId19"/>
     <sheet name="ServicedEntity" sheetId="24" r:id="rId20"/>
     <sheet name="ReviewCharges" sheetId="26" r:id="rId21"/>
-    <sheet name="Sheet7" sheetId="25" r:id="rId22"/>
-    <sheet name="ReceiveAdjust" sheetId="13" r:id="rId23"/>
-    <sheet name="TransferAdjust" sheetId="14" r:id="rId24"/>
-    <sheet name="DestroyAdjust" sheetId="15" r:id="rId25"/>
-    <sheet name="ReturnToSupplierAdjust" sheetId="16" r:id="rId26"/>
+    <sheet name="ReceiveAdjust" sheetId="13" r:id="rId22"/>
+    <sheet name="TransferAdjust" sheetId="14" r:id="rId23"/>
+    <sheet name="DestroyAdjust" sheetId="15" r:id="rId24"/>
+    <sheet name="ReturnToSupplierAdjust" sheetId="16" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="559">
   <si>
     <t>UserName</t>
   </si>
@@ -1237,9 +1236,6 @@
     <t>Patient_Study_ID</t>
   </si>
   <si>
-    <t>QWERT-U-02</t>
-  </si>
-  <si>
     <t>ZAP-U1-</t>
   </si>
   <si>
@@ -1603,15 +1599,6 @@
     <t>Billable</t>
   </si>
   <si>
-    <t>Non Billable</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t>Hold</t>
-  </si>
-  <si>
     <t>review-charges-drug</t>
   </si>
   <si>
@@ -1645,12 +1632,6 @@
     <t>07302020</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Class88765</t>
-  </si>
-  <si>
     <t>dispense-protocol</t>
   </si>
   <si>
@@ -1681,67 +1662,79 @@
     <t>ZAP-U1-0018</t>
   </si>
   <si>
-    <t>13-JUL-01-20-PROT</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-Supplier-1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>13-JUL-01-Supplier-2</t>
-  </si>
-  <si>
-    <t>13-JUL-01-Supplier-3</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-FN</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-LN</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-Unit 22.22mEq</t>
-  </si>
-  <si>
-    <t>13-JUL-01-20-Drg-Unit 22.22 mEq(Enema)</t>
-  </si>
-  <si>
-    <t>ncoup</t>
+    <t>ncoup123</t>
+  </si>
+  <si>
+    <t>01-JUN-Payer-IDS</t>
+  </si>
+  <si>
+    <t>01-JUN-Payer-Name</t>
+  </si>
+  <si>
+    <t>QWERT-LT-01</t>
+  </si>
+  <si>
+    <t>25-JUL-09-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PROT</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-Supplier-1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-12-Supplier-2</t>
+  </si>
+  <si>
+    <t>25-JUL-12-Supplier-3</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-FN</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-LN</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-Unit 22.22mEq</t>
+  </si>
+  <si>
+    <t>25-JUL-12-20-Drg-Unit 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -2065,6 +2058,33 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2082,33 +2102,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2998,16 +2991,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3046,51 +3039,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="53" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="55"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="46"/>
       <c r="AB7" s="47" t="s">
         <v>143</v>
       </c>
@@ -3262,10 +3255,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>540</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>541</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3274,10 +3267,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>542</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>543</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3401,80 +3394,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="50"/>
-      <c r="AC12" s="50"/>
-      <c r="AD12" s="50"/>
-      <c r="AE12" s="50"/>
-      <c r="AF12" s="50"/>
-      <c r="AG12" s="50" t="s">
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50"/>
-      <c r="AJ12" s="50"/>
-      <c r="AK12" s="50"/>
-      <c r="AL12" s="50"/>
-      <c r="AM12" s="50" t="s">
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="43"/>
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="50"/>
-      <c r="AO12" s="50"/>
-      <c r="AP12" s="50"/>
-      <c r="AQ12" s="50"/>
-      <c r="AR12" s="50"/>
-      <c r="AS12" s="50"/>
-      <c r="AT12" s="50"/>
-      <c r="AU12" s="50"/>
-      <c r="AV12" s="50"/>
-      <c r="AW12" s="50"/>
-      <c r="AX12" s="50"/>
-      <c r="AY12" s="50"/>
-      <c r="AZ12" s="50"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="43"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="43"/>
+      <c r="AU12" s="43"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
+      <c r="AX12" s="43"/>
+      <c r="AY12" s="43"/>
+      <c r="AZ12" s="43"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3637,7 +3630,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3652,16 +3645,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>544</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>547</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>548</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3685,13 +3678,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3724,10 +3717,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -3780,7 +3773,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>13-JUL-01-20-Drg-Unit 22.22 mEq</v>
+        <v>25-JUL-12-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -3796,16 +3789,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -3830,16 +3823,16 @@
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
       <c r="P17" s="49"/>
-      <c r="Q17" s="50" t="s">
+      <c r="Q17" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="50"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="43"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -3924,7 +3917,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4027,29 +4020,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>551</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4065,48 +4058,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="55"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50" t="s">
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4185,13 +4178,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>553</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>554</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>555</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4203,13 +4196,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>556</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>557</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4257,16 +4250,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="52"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4342,10 +4335,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4386,16 +4379,16 @@
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="46"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="55"/>
     </row>
     <row r="37" spans="1:21" ht="58.2" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
@@ -4438,16 +4431,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C38" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>226</v>
@@ -4495,16 +4488,16 @@
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="52"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
@@ -4530,16 +4523,16 @@
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="43"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="52"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
@@ -4773,19 +4766,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -4798,6 +4778,19 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B36:I36"/>
     <mergeCell ref="B41:I41"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -4812,7 +4805,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4882,10 +4875,10 @@
     </row>
     <row r="2" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -4897,16 +4890,16 @@
         <v>23232</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>392</v>
+        <v>537</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>226</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>252</v>
+        <v>538</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>226</v>
@@ -4915,11 +4908,11 @@
         <v>251</v>
       </c>
       <c r="L2" s="14">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -4938,7 +4931,7 @@
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4952,177 +4945,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="R1" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="B1" t="s">
-        <v>531</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="17" t="s">
         <v>415</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="17" t="s">
         <v>417</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="17" t="s">
         <v>418</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="17" t="s">
         <v>419</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="17" t="s">
         <v>421</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="17" t="s">
         <v>423</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>427</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="17" t="s">
         <v>434</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>436</v>
-      </c>
     </row>
     <row r="2" spans="1:44" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>540</v>
-      </c>
-      <c r="B2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C2" t="s">
-        <v>558</v>
-      </c>
-      <c r="D2" t="s">
-        <v>392</v>
-      </c>
-      <c r="J2" t="s">
-        <v>252</v>
-      </c>
-      <c r="K2" t="s">
-        <v>225</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="A2" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="L2" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="M2" t="s">
-        <v>532</v>
-      </c>
-      <c r="P2" t="s">
-        <v>534</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="M2" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="R2" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="R2" t="s">
-        <v>539</v>
-      </c>
-      <c r="S2">
-        <v>4</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="S2" s="14">
+        <v>5</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>387</v>
       </c>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:AR1">
@@ -5147,22 +5171,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -5188,46 +5212,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -5253,37 +5277,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -5302,7 +5326,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5313,18 +5337,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -5343,112 +5367,113 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B2" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D2" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="F2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="J2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="40" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="R2" s="40" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -5474,31 +5499,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -5514,20 +5539,28 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14682C1A-A86D-4C5D-B3D9-0D5F958B3EAC}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>497</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -5553,25 +5586,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -5622,10 +5655,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" t="s">
         <v>394</v>
-      </c>
-      <c r="B1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5663,39 +5696,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E2" t="s">
         <v>511</v>
-      </c>
-      <c r="E2" t="s">
-        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -5729,42 +5762,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D2" s="38">
         <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F2" t="s">
         <v>512</v>
-      </c>
-      <c r="F2" t="s">
-        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -5779,47 +5812,21 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D031FBF6-64A1-4FBB-B36B-C5EBC575879C}">
-  <dimension ref="B3:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8726B607-4FF5-4DF0-BBA1-3FCDBD3D0C76}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>511</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8726B607-4FF5-4DF0-BBA1-3FCDBD3D0C76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428AC387-3CDC-4E5F-B0D8-F4C06660CF08}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5831,10 +5838,12 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428AC387-3CDC-4E5F-B0D8-F4C06660CF08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD543CE2-8AA7-4742-B4D5-FFAFE66E2413}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -5843,18 +5852,6 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD543CE2-8AA7-4742-B4D5-FFAFE66E2413}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3F60D2-8704-4C3A-987D-064E20473D5E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5872,7 +5869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E176A9F-48C8-4663-B776-82E4899D5865}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5885,7 +5882,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -5899,13 +5896,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>387</v>
@@ -5930,7 +5927,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6053,7 +6050,7 @@
         <v>293</v>
       </c>
       <c r="AJ1" s="29" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="AK1" s="29" t="s">
         <v>294</v>
@@ -6076,10 +6073,10 @@
     </row>
     <row r="2" spans="1:42" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>540</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>541</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>152</v>
@@ -6088,10 +6085,10 @@
         <v>153</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>542</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>543</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>231</v>
@@ -6179,7 +6176,7 @@
         <v>180</v>
       </c>
       <c r="AJ2" s="17" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="AK2" s="17" t="s">
         <v>181</v>
@@ -6210,8 +6207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B189598-4DA9-43C3-A7E7-FA94EEA5CFDF}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6302,7 +6299,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>192</v>
@@ -6344,7 +6341,7 @@
         <v>229</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="Q2" s="17">
         <v>11</v>
@@ -6384,7 +6381,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6418,13 +6415,13 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>551</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>387</v>
@@ -6441,7 +6438,7 @@
   <dimension ref="A1:AY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6606,7 +6603,7 @@
     </row>
     <row r="2" spans="1:51" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>188</v>
@@ -6621,16 +6618,16 @@
         <v>190</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>544</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>547</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>548</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>191</v>
@@ -6645,7 +6642,7 @@
         <v>192</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>194</v>
@@ -6654,13 +6651,13 @@
         <v>48</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="R2" s="17" t="s">
         <v>222</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="T2" s="17" t="s">
         <v>226</v>
@@ -6693,10 +6690,10 @@
       <c r="AD2" s="22"/>
       <c r="AE2" s="22"/>
       <c r="AF2" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AH2" s="22"/>
       <c r="AI2" s="22"/>
@@ -6755,8 +6752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CE59FD-224B-4A01-AB17-7B870C2F09CB}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6847,13 +6844,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>553</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>554</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>555</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -6865,13 +6862,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>556</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>557</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -6931,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFFB398-D4A3-48F4-A43E-4EBC96369A2B}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7016,10 +7013,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E2" s="23">
         <v>22.22</v>
@@ -7033,7 +7030,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>392</v>
+        <v>537</v>
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
@@ -7043,7 +7040,9 @@
         <v>232</v>
       </c>
       <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="Q2" s="14">
+        <v>25</v>
+      </c>
       <c r="R2" s="14">
         <v>209</v>
       </c>
@@ -7051,7 +7050,7 @@
         <v>233</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="U2" s="14">
         <v>10</v>

</xml_diff>

<commit_message>
committing on 25-JUL-20 part 2
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25380EB-FFB6-47D4-8E40-A8495180E452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E596E05E-487E-4A5A-A094-5B426EB7220D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="5" activeTab="9" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1674,67 +1674,67 @@
     <t>QWERT-LT-01</t>
   </si>
   <si>
-    <t>25-JUL-09-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PROT</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-Supplier-1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>25-JUL-12-Supplier-2</t>
-  </si>
-  <si>
-    <t>25-JUL-12-Supplier-3</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-FN</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-LN</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-Unit 22.22mEq</t>
-  </si>
-  <si>
-    <t>25-JUL-12-20-Drg-Unit 22.22 mEq(Enema)</t>
+    <t>25-JUL-10-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PROT</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-Supplier-1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-13-Supplier-2</t>
+  </si>
+  <si>
+    <t>25-JUL-13-Supplier-3</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-FN</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-LN</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-Unit 22.22mEq</t>
+  </si>
+  <si>
+    <t>25-JUL-13-20-Drg-Unit 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -2058,33 +2058,6 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2102,6 +2075,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2991,16 +2991,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3039,51 +3039,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="44" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="46"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="55"/>
       <c r="AB7" s="47" t="s">
         <v>143</v>
       </c>
@@ -3394,80 +3394,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="43"/>
-      <c r="AF12" s="43"/>
-      <c r="AG12" s="43" t="s">
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
+      <c r="AC12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="43"/>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
-      <c r="AL12" s="43"/>
-      <c r="AM12" s="43" t="s">
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="43"/>
-      <c r="AO12" s="43"/>
-      <c r="AP12" s="43"/>
-      <c r="AQ12" s="43"/>
-      <c r="AR12" s="43"/>
-      <c r="AS12" s="43"/>
-      <c r="AT12" s="43"/>
-      <c r="AU12" s="43"/>
-      <c r="AV12" s="43"/>
-      <c r="AW12" s="43"/>
-      <c r="AX12" s="43"/>
-      <c r="AY12" s="43"/>
-      <c r="AZ12" s="43"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="50"/>
+      <c r="AR12" s="50"/>
+      <c r="AS12" s="50"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="50"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>25-JUL-12-20-Drg-Unit 22.22 mEq</v>
+        <v>25-JUL-13-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -3789,16 +3789,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -3823,16 +3823,16 @@
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
       <c r="P17" s="49"/>
-      <c r="Q17" s="43" t="s">
+      <c r="Q17" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="43"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -4033,16 +4033,16 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4058,48 +4058,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="55"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4250,16 +4250,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="52"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4379,16 +4379,16 @@
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="46"/>
     </row>
     <row r="37" spans="1:21" ht="58.2" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
@@ -4488,16 +4488,16 @@
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="52"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
@@ -4523,16 +4523,16 @@
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="52"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="43"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
@@ -4766,6 +4766,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -4778,19 +4791,6 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B36:I36"/>
     <mergeCell ref="B41:I41"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -4804,8 +4804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D9EE97-5104-41E4-A9AA-9141C3852F0E}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4931,7 +4931,7 @@
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6752,7 +6752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CE59FD-224B-4A01-AB17-7B870C2F09CB}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
committing on 25-JUL-20 part 3
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E596E05E-487E-4A5A-A094-5B426EB7220D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB64B091-BD41-47D7-86A0-A078F1AE7D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="5" activeTab="9" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1677,64 +1677,64 @@
     <t>25-JUL-10-20-Pharm1-C</t>
   </si>
   <si>
-    <t>25-JUL-13-20-PROT</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-Supplier-1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>25-JUL-13-Supplier-2</t>
-  </si>
-  <si>
-    <t>25-JUL-13-Supplier-3</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-FN</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-LN</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-Unit 22.22mEq</t>
-  </si>
-  <si>
-    <t>25-JUL-13-20-Drg-Unit 22.22 mEq(Enema)</t>
+    <t>25-JUL-14-20-PROT</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-Supplier-1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-14-Supplier-2</t>
+  </si>
+  <si>
+    <t>25-JUL-14-Supplier-3</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-FN</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-LN</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-Unit 22.22mEq</t>
+  </si>
+  <si>
+    <t>25-JUL-14-20-Drg-Unit 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -2058,6 +2058,33 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2075,33 +2102,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2991,16 +2991,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3039,51 +3039,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="53" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="55"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="46"/>
       <c r="AB7" s="47" t="s">
         <v>143</v>
       </c>
@@ -3394,80 +3394,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="50"/>
-      <c r="AC12" s="50"/>
-      <c r="AD12" s="50"/>
-      <c r="AE12" s="50"/>
-      <c r="AF12" s="50"/>
-      <c r="AG12" s="50" t="s">
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50"/>
-      <c r="AJ12" s="50"/>
-      <c r="AK12" s="50"/>
-      <c r="AL12" s="50"/>
-      <c r="AM12" s="50" t="s">
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="43"/>
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="50"/>
-      <c r="AO12" s="50"/>
-      <c r="AP12" s="50"/>
-      <c r="AQ12" s="50"/>
-      <c r="AR12" s="50"/>
-      <c r="AS12" s="50"/>
-      <c r="AT12" s="50"/>
-      <c r="AU12" s="50"/>
-      <c r="AV12" s="50"/>
-      <c r="AW12" s="50"/>
-      <c r="AX12" s="50"/>
-      <c r="AY12" s="50"/>
-      <c r="AZ12" s="50"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="43"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="43"/>
+      <c r="AU12" s="43"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
+      <c r="AX12" s="43"/>
+      <c r="AY12" s="43"/>
+      <c r="AZ12" s="43"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>25-JUL-13-20-Drg-Unit 22.22 mEq</v>
+        <v>25-JUL-14-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -3789,16 +3789,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -3823,16 +3823,16 @@
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
       <c r="P17" s="49"/>
-      <c r="Q17" s="50" t="s">
+      <c r="Q17" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="50"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="43"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -4033,16 +4033,16 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4058,48 +4058,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="55"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50" t="s">
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4250,16 +4250,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="52"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4379,16 +4379,16 @@
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="46"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="55"/>
     </row>
     <row r="37" spans="1:21" ht="58.2" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
@@ -4488,16 +4488,16 @@
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="52"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
@@ -4523,16 +4523,16 @@
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="43"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="52"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
@@ -4766,19 +4766,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -4791,6 +4778,19 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B36:I36"/>
     <mergeCell ref="B41:I41"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -4805,7 +4805,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 25-JUL-20 part 4
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB64B091-BD41-47D7-86A0-A078F1AE7D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0559830C-5F7D-4499-97DF-976491BE82A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="5" activeTab="9" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1677,64 +1677,64 @@
     <t>25-JUL-10-20-Pharm1-C</t>
   </si>
   <si>
-    <t>25-JUL-14-20-PROT</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-Supplier-1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>25-JUL-14-Supplier-2</t>
-  </si>
-  <si>
-    <t>25-JUL-14-Supplier-3</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-FN</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-LN</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-Unit 22.22mEq</t>
-  </si>
-  <si>
-    <t>25-JUL-14-20-Drg-Unit 22.22 mEq(Enema)</t>
+    <t>25-JUL-15-20-PROT</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-Supplier-1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>25-JUL-15-Supplier-2</t>
+  </si>
+  <si>
+    <t>25-JUL-15-Supplier-3</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-FN</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-LN</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-Unit 22.22mEq</t>
+  </si>
+  <si>
+    <t>25-JUL-15-20-Drg-Unit 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -2058,33 +2058,6 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2102,6 +2075,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2991,16 +2991,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3039,51 +3039,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="44" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="46"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="55"/>
       <c r="AB7" s="47" t="s">
         <v>143</v>
       </c>
@@ -3394,80 +3394,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="43"/>
-      <c r="AF12" s="43"/>
-      <c r="AG12" s="43" t="s">
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
+      <c r="AC12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="43"/>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
-      <c r="AL12" s="43"/>
-      <c r="AM12" s="43" t="s">
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="43"/>
-      <c r="AO12" s="43"/>
-      <c r="AP12" s="43"/>
-      <c r="AQ12" s="43"/>
-      <c r="AR12" s="43"/>
-      <c r="AS12" s="43"/>
-      <c r="AT12" s="43"/>
-      <c r="AU12" s="43"/>
-      <c r="AV12" s="43"/>
-      <c r="AW12" s="43"/>
-      <c r="AX12" s="43"/>
-      <c r="AY12" s="43"/>
-      <c r="AZ12" s="43"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="50"/>
+      <c r="AR12" s="50"/>
+      <c r="AS12" s="50"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="50"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>25-JUL-14-20-Drg-Unit 22.22 mEq</v>
+        <v>25-JUL-15-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -3789,16 +3789,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -3823,16 +3823,16 @@
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
       <c r="P17" s="49"/>
-      <c r="Q17" s="43" t="s">
+      <c r="Q17" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="43"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -4033,16 +4033,16 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4058,48 +4058,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="55"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4250,16 +4250,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="52"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4379,16 +4379,16 @@
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="46"/>
     </row>
     <row r="37" spans="1:21" ht="58.2" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
@@ -4488,16 +4488,16 @@
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="52"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
@@ -4523,16 +4523,16 @@
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="52"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="43"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
@@ -4766,6 +4766,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -4778,19 +4791,6 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B36:I36"/>
     <mergeCell ref="B41:I41"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -4805,7 +4805,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 2
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF85575-EE6B-4280-8FDB-4375A5FC7E38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03805CA-0ED9-4117-8E18-9C9A5DB05478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="6" activeTab="8" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="12" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1625,12 +1625,6 @@
     <t>cpp-cdm-price-eff-to</t>
   </si>
   <si>
-    <t>06302020</t>
-  </si>
-  <si>
-    <t>07302020</t>
-  </si>
-  <si>
     <t>dispense-protocol</t>
   </si>
   <si>
@@ -1898,91 +1892,97 @@
     <t>586.iu45-LT3</t>
   </si>
   <si>
-    <t>28-SEP-01-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-01-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-01-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-01-20-Drg 22.22 mEq(Enema)</t>
+    <t>30-Sep-2020</t>
+  </si>
+  <si>
+    <t>28-Sep-2020</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-02-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-02-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-02-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -2319,6 +2319,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2336,33 +2363,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3252,16 +3252,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3300,51 +3300,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="56" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="57"/>
-      <c r="AA7" s="58"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="49"/>
       <c r="AB7" s="50" t="s">
         <v>143</v>
       </c>
@@ -3655,80 +3655,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="53"/>
-      <c r="Y12" s="53"/>
-      <c r="Z12" s="53"/>
-      <c r="AA12" s="53"/>
-      <c r="AB12" s="53"/>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="53"/>
-      <c r="AE12" s="53"/>
-      <c r="AF12" s="53"/>
-      <c r="AG12" s="53" t="s">
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="46"/>
+      <c r="AB12" s="46"/>
+      <c r="AC12" s="46"/>
+      <c r="AD12" s="46"/>
+      <c r="AE12" s="46"/>
+      <c r="AF12" s="46"/>
+      <c r="AG12" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="53"/>
-      <c r="AI12" s="53"/>
-      <c r="AJ12" s="53"/>
-      <c r="AK12" s="53"/>
-      <c r="AL12" s="53"/>
-      <c r="AM12" s="53" t="s">
+      <c r="AH12" s="46"/>
+      <c r="AI12" s="46"/>
+      <c r="AJ12" s="46"/>
+      <c r="AK12" s="46"/>
+      <c r="AL12" s="46"/>
+      <c r="AM12" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="53"/>
-      <c r="AO12" s="53"/>
-      <c r="AP12" s="53"/>
-      <c r="AQ12" s="53"/>
-      <c r="AR12" s="53"/>
-      <c r="AS12" s="53"/>
-      <c r="AT12" s="53"/>
-      <c r="AU12" s="53"/>
-      <c r="AV12" s="53"/>
-      <c r="AW12" s="53"/>
-      <c r="AX12" s="53"/>
-      <c r="AY12" s="53"/>
-      <c r="AZ12" s="53"/>
+      <c r="AN12" s="46"/>
+      <c r="AO12" s="46"/>
+      <c r="AP12" s="46"/>
+      <c r="AQ12" s="46"/>
+      <c r="AR12" s="46"/>
+      <c r="AS12" s="46"/>
+      <c r="AT12" s="46"/>
+      <c r="AU12" s="46"/>
+      <c r="AV12" s="46"/>
+      <c r="AW12" s="46"/>
+      <c r="AX12" s="46"/>
+      <c r="AY12" s="46"/>
+      <c r="AZ12" s="46"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-01-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-02-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4050,16 +4050,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -4084,16 +4084,16 @@
       <c r="N17" s="51"/>
       <c r="O17" s="51"/>
       <c r="P17" s="52"/>
-      <c r="Q17" s="53" t="s">
+      <c r="Q17" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -4294,16 +4294,16 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="55"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4319,48 +4319,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="49"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="53"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4511,16 +4511,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="55"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4639,19 +4639,19 @@
         <v>3</v>
       </c>
       <c r="E35" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="H35" s="31" t="s">
         <v>590</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="I35" s="13" t="s">
         <v>591</v>
-      </c>
-      <c r="H35" s="31" t="s">
-        <v>592</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>593</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>31</v>
@@ -4671,13 +4671,13 @@
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
       <c r="D36" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>193</v>
@@ -4687,10 +4687,10 @@
         <v>300</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L36" s="40"/>
       <c r="M36" s="43"/>
@@ -4841,16 +4841,16 @@
       <c r="A45" s="6">
         <v>35</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="49"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="58"/>
     </row>
     <row r="46" spans="1:21" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
@@ -4950,16 +4950,16 @@
       <c r="A50" s="6">
         <v>40</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="46"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="55"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
@@ -4985,16 +4985,16 @@
       <c r="A55" s="6">
         <v>45</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="46"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="54"/>
+      <c r="I55" s="55"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
@@ -5228,19 +5228,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B55:I55"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -5253,6 +5240,19 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B45:I45"/>
     <mergeCell ref="B50:I50"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -5548,7 +5548,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>193</v>
@@ -5570,7 +5570,7 @@
         <v>233</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="U2" s="14">
         <v>99</v>
@@ -5679,7 +5679,7 @@
         <v>629</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>631</v>
@@ -5688,7 +5688,7 @@
         <v>227</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>227</v>
@@ -5701,7 +5701,7 @@
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -5737,10 +5737,10 @@
   <sheetData>
     <row r="1" spans="1:44" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>396</v>
@@ -5788,7 +5788,7 @@
         <v>410</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="S1" s="17" t="s">
         <v>411</v>
@@ -5797,7 +5797,7 @@
         <v>412</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="V1" s="17"/>
       <c r="W1" s="17" t="s">
@@ -5878,7 +5878,7 @@
         <v>639</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5886,7 +5886,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>223</v>
@@ -5895,18 +5895,18 @@
         <v>227</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Q2" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="R2" s="14" t="s">
         <v>607</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>609</v>
       </c>
       <c r="S2" s="14">
         <v>9</v>
@@ -6157,8 +6157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E63512-8B54-43D1-9A38-91DAF3F128E4}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6237,10 +6237,10 @@
         <v>612</v>
       </c>
       <c r="B2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F2" t="s">
         <v>514</v>
@@ -6261,10 +6261,10 @@
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>521</v>
+        <v>611</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>522</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -6373,386 +6373,386 @@
     </row>
     <row r="7" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C7" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D7" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E7" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G7" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H7" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I7" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J7" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I8" t="s">
+        <v>537</v>
+      </c>
+      <c r="J8" t="s">
         <v>539</v>
-      </c>
-      <c r="J8" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="288" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D9" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E9" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F9" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G9" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H9" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I9" t="s">
+        <v>537</v>
+      </c>
+      <c r="J9" t="s">
         <v>539</v>
-      </c>
-      <c r="J9" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C10" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D10" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E10" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F10" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G10" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H10" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I10" t="s">
+        <v>537</v>
+      </c>
+      <c r="J10" t="s">
         <v>539</v>
-      </c>
-      <c r="J10" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H11" t="s">
+        <v>579</v>
+      </c>
+      <c r="I11" t="s">
         <v>581</v>
       </c>
-      <c r="I11" t="s">
-        <v>583</v>
-      </c>
       <c r="J11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C12" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G12" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H12" t="s">
+        <v>579</v>
+      </c>
+      <c r="I12" t="s">
         <v>581</v>
       </c>
-      <c r="I12" t="s">
-        <v>583</v>
-      </c>
       <c r="J12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C13" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D13" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E13" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F13" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I13" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J13" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F14" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G14" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J14" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C15" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D15" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E15" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H15" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I15" t="s">
+        <v>537</v>
+      </c>
+      <c r="J15" t="s">
         <v>539</v>
-      </c>
-      <c r="J15" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C16" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D16" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E16" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G16" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H16" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I16" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J16" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C17" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G17" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H17" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I17" t="s">
+        <v>537</v>
+      </c>
+      <c r="J17" t="s">
         <v>539</v>
-      </c>
-      <c r="J17" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C18" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F18" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G18" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H18" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I18" t="s">
+        <v>537</v>
+      </c>
+      <c r="J18" t="s">
         <v>539</v>
-      </c>
-      <c r="J18" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7058,156 +7058,156 @@
         <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B10" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B18" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -7234,16 +7234,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
+        <v>529</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="D1" s="13" t="s">
         <v>532</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>533</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>534</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>94</v>
@@ -7255,45 +7255,45 @@
         <v>95</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -7339,7 +7339,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>387</v>
@@ -7389,7 +7389,7 @@
         <v>263</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>264</v>
@@ -7491,7 +7491,7 @@
         <v>293</v>
       </c>
       <c r="AK1" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AL1" s="29" t="s">
         <v>294</v>
@@ -7620,7 +7620,7 @@
         <v>180</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AL2" s="17" t="s">
         <v>181</v>
@@ -7669,7 +7669,7 @@
         <v>295</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>296</v>
@@ -7853,7 +7853,7 @@
         <v>319</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>320</v>
@@ -7895,8 +7895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C02648-616D-42A5-9175-58AAD7AE2F9C}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7912,7 +7912,7 @@
         <v>322</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>323</v>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 3
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03805CA-0ED9-4117-8E18-9C9A5DB05478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85DFB60-DEDA-480A-A955-EE626DB33814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="12" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1898,91 +1898,91 @@
     <t>28-Sep-2020</t>
   </si>
   <si>
-    <t>28-SEP-02-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-02-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-02-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-02-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-03-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-03-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-03-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-03-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-02-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-03-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -6158,7 +6158,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 5
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A87CE6B-2B73-4615-82C3-30ED13CBD994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F4EC55-1E19-4EAB-88DF-B5784A65AF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="640">
   <si>
     <t>UserName</t>
   </si>
@@ -1868,9 +1868,6 @@
     <t>Supplier_Name_1_Edit</t>
   </si>
   <si>
-    <t>586.iu45-LT2</t>
-  </si>
-  <si>
     <t>6 tabs twice a day</t>
   </si>
   <si>
@@ -1898,91 +1895,91 @@
     <t>28-Sep-2020</t>
   </si>
   <si>
-    <t>28-SEP-04-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-04-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-04-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-04-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-05-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-05-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-05-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-05-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -3516,10 +3513,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>612</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>613</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3528,10 +3525,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>613</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>615</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3891,7 +3888,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3906,16 +3903,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>616</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>617</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>618</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>619</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>620</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3939,13 +3936,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3978,10 +3975,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4034,7 +4031,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-04-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-05-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4178,7 +4175,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4281,13 +4278,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>623</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4439,13 +4436,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>626</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>627</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4457,13 +4454,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>628</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>629</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4596,10 +4593,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4893,16 +4890,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5360,13 +5357,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>626</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>627</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5378,13 +5375,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>628</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>629</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5444,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFFB398-D4A3-48F4-A43E-4EBC96369A2B}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5531,10 +5528,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5548,7 +5545,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>193</v>
@@ -5592,7 +5589,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5664,10 +5661,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5676,19 +5673,19 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>227</v>
@@ -5701,7 +5698,7 @@
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -5719,8 +5716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66856262-9FC7-44EB-98DF-8D229C6B1BEB}">
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5869,16 +5866,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5886,7 +5883,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>223</v>
@@ -5895,18 +5892,18 @@
         <v>227</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q2" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="Q2" s="14" t="s">
-        <v>605</v>
-      </c>
       <c r="R2" s="14" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S2" s="14">
         <v>9</v>
@@ -6136,10 +6133,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -6157,8 +6154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E63512-8B54-43D1-9A38-91DAF3F128E4}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6234,7 +6231,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B2" t="s">
         <v>527</v>
@@ -6255,16 +6252,16 @@
         <v>516</v>
       </c>
       <c r="J2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -6793,7 +6790,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6889,13 +6886,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -6955,13 +6952,13 @@
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D2" s="37">
         <v>20</v>
@@ -7339,7 +7336,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>387</v>
@@ -7514,13 +7511,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>611</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>612</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>613</v>
-      </c>
       <c r="C2" s="17" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7529,10 +7526,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
+        <v>613</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>615</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7746,10 +7743,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>631</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>632</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7870,16 +7867,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>634</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>635</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>636</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -8067,10 +8064,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8085,16 +8082,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I2" s="20" t="s">
+        <v>618</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>619</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>620</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8118,13 +8115,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8157,10 +8154,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 6
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F4EC55-1E19-4EAB-88DF-B5784A65AF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029A2020-B22B-4AC5-B469-020E775CE5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="8" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1895,91 +1895,91 @@
     <t>28-Sep-2020</t>
   </si>
   <si>
-    <t>28-SEP-05-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-05-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-05-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-05-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-06-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-06-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-06-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-06-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-05-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-06-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -5442,7 +5442,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5589,7 +5589,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5717,7 +5717,7 @@
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5993,7 +5993,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 7
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029A2020-B22B-4AC5-B469-020E775CE5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A9BEA-EF9C-4015-9972-F9F9FA49C404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="8" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1895,91 +1895,91 @@
     <t>28-Sep-2020</t>
   </si>
   <si>
-    <t>28-SEP-06-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-06-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-06-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-06-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-07-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-07-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-07-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-07-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-06-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-07-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -5442,7 +5442,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 8
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A9BEA-EF9C-4015-9972-F9F9FA49C404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E785E-CB79-4548-977F-C12EE7D8F725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="8" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="16" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="639">
   <si>
     <t>UserName</t>
   </si>
@@ -1604,9 +1604,6 @@
     <t>review-charges-price</t>
   </si>
   <si>
-    <t>12345Name</t>
-  </si>
-  <si>
     <t>Study Team</t>
   </si>
   <si>
@@ -1643,12 +1640,6 @@
     <t>Patient Returns Notifications</t>
   </si>
   <si>
-    <t>01-JUN-Payer-IDS</t>
-  </si>
-  <si>
-    <t>01-JUN-Payer-Name</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -1895,91 +1886,97 @@
     <t>28-Sep-2020</t>
   </si>
   <si>
-    <t>28-SEP-07-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-07-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-07-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-07-20-Drg 22.22 mEq(Enema)</t>
+    <t>Dummil-Test</t>
+  </si>
+  <si>
+    <t>12345Dummil</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-08-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-08-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-08-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -3513,10 +3510,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>610</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>611</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>612</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3525,10 +3522,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>612</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>613</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>614</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3888,7 +3885,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3903,16 +3900,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>615</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>617</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>618</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>619</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3936,13 +3933,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3975,10 +3972,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4031,7 +4028,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-07-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-08-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4175,7 +4172,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4278,13 +4275,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>622</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4436,13 +4433,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>624</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>625</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>626</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4454,13 +4451,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>627</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>628</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4593,10 +4590,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4636,19 +4633,19 @@
         <v>3</v>
       </c>
       <c r="E35" s="13" t="s">
+        <v>584</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>585</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="H35" s="31" t="s">
         <v>587</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="I35" s="13" t="s">
         <v>588</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>589</v>
-      </c>
-      <c r="H35" s="31" t="s">
-        <v>590</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>591</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>31</v>
@@ -4668,13 +4665,13 @@
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
       <c r="D36" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>592</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>596</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>595</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>193</v>
@@ -4684,10 +4681,10 @@
         <v>300</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="L36" s="40"/>
       <c r="M36" s="43"/>
@@ -4890,16 +4887,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5357,13 +5354,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>625</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>626</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5375,13 +5372,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>627</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>628</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5441,7 +5438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFFB398-D4A3-48F4-A43E-4EBC96369A2B}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -5528,10 +5525,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5545,7 +5542,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>193</v>
@@ -5567,7 +5564,7 @@
         <v>233</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="U2" s="14">
         <v>99</v>
@@ -5661,10 +5658,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5673,19 +5670,19 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>227</v>
@@ -5698,7 +5695,7 @@
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -5734,10 +5731,10 @@
   <sheetData>
     <row r="1" spans="1:44" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>521</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>522</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>396</v>
@@ -5785,7 +5782,7 @@
         <v>410</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="S1" s="17" t="s">
         <v>411</v>
@@ -5794,7 +5791,7 @@
         <v>412</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V1" s="17"/>
       <c r="W1" s="17" t="s">
@@ -5866,16 +5863,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5883,7 +5880,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>223</v>
@@ -5892,18 +5889,18 @@
         <v>227</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="R2" s="14" t="s">
         <v>603</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>604</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>606</v>
       </c>
       <c r="S2" s="14">
         <v>9</v>
@@ -6114,7 +6111,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6133,10 +6130,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -6154,13 +6151,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E63512-8B54-43D1-9A38-91DAF3F128E4}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
@@ -6196,7 +6193,7 @@
         <v>476</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>477</v>
@@ -6217,10 +6214,10 @@
         <v>482</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>520</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>483</v>
@@ -6231,37 +6228,37 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
-        <v>527</v>
+        <v>608</v>
       </c>
       <c r="D2" t="s">
-        <v>528</v>
+        <v>608</v>
       </c>
       <c r="F2" t="s">
+        <v>609</v>
+      </c>
+      <c r="G2" t="s">
         <v>514</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="38" t="s">
+        <v>516</v>
+      </c>
+      <c r="I2" t="s">
         <v>515</v>
       </c>
-      <c r="H2" s="38" t="s">
-        <v>517</v>
-      </c>
-      <c r="I2" t="s">
-        <v>516</v>
-      </c>
       <c r="J2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
   </sheetData>
@@ -6370,386 +6367,386 @@
     </row>
     <row r="7" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C7" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F7" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G7" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H7" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I7" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C8" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D8" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E8" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F8" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G8" t="s">
+        <v>531</v>
+      </c>
+      <c r="H8" t="s">
+        <v>577</v>
+      </c>
+      <c r="I8" t="s">
         <v>534</v>
       </c>
-      <c r="H8" t="s">
-        <v>580</v>
-      </c>
-      <c r="I8" t="s">
-        <v>537</v>
-      </c>
       <c r="J8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="288" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C9" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D9" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E9" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F9" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G9" t="s">
+        <v>531</v>
+      </c>
+      <c r="H9" t="s">
+        <v>577</v>
+      </c>
+      <c r="I9" t="s">
         <v>534</v>
       </c>
-      <c r="H9" t="s">
-        <v>580</v>
-      </c>
-      <c r="I9" t="s">
-        <v>537</v>
-      </c>
       <c r="J9" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C10" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D10" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E10" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F10" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G10" t="s">
+        <v>531</v>
+      </c>
+      <c r="H10" t="s">
+        <v>577</v>
+      </c>
+      <c r="I10" t="s">
         <v>534</v>
       </c>
-      <c r="H10" t="s">
-        <v>580</v>
-      </c>
-      <c r="I10" t="s">
-        <v>537</v>
-      </c>
       <c r="J10" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C11" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D11" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E11" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F11" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G11" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H11" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I11" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J11" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C12" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D12" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E12" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F12" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G12" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H12" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I12" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C13" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D13" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E13" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F13" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G13" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H13" t="s">
+        <v>576</v>
+      </c>
+      <c r="I13" t="s">
         <v>579</v>
       </c>
-      <c r="I13" t="s">
-        <v>582</v>
-      </c>
       <c r="J13" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C14" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F14" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G14" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H14" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I14" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J14" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F15" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G15" t="s">
+        <v>531</v>
+      </c>
+      <c r="H15" t="s">
+        <v>577</v>
+      </c>
+      <c r="I15" t="s">
         <v>534</v>
       </c>
-      <c r="H15" t="s">
-        <v>580</v>
-      </c>
-      <c r="I15" t="s">
-        <v>537</v>
-      </c>
       <c r="J15" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C16" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D16" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E16" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F16" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="G16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H16" t="s">
+        <v>576</v>
+      </c>
+      <c r="I16" t="s">
         <v>579</v>
       </c>
-      <c r="I16" t="s">
-        <v>582</v>
-      </c>
       <c r="J16" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C17" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D17" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E17" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F17" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G17" t="s">
+        <v>531</v>
+      </c>
+      <c r="H17" t="s">
+        <v>577</v>
+      </c>
+      <c r="I17" t="s">
         <v>534</v>
       </c>
-      <c r="H17" t="s">
-        <v>580</v>
-      </c>
-      <c r="I17" t="s">
-        <v>537</v>
-      </c>
       <c r="J17" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C18" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D18" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E18" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F18" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G18" t="s">
+        <v>531</v>
+      </c>
+      <c r="H18" t="s">
+        <v>577</v>
+      </c>
+      <c r="I18" t="s">
         <v>534</v>
       </c>
-      <c r="H18" t="s">
-        <v>580</v>
-      </c>
-      <c r="I18" t="s">
-        <v>537</v>
-      </c>
       <c r="J18" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6790,7 +6787,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6810,7 +6807,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6886,13 +6883,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -6952,13 +6949,13 @@
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D2" s="37">
         <v>20</v>
@@ -7055,156 +7052,156 @@
         <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F2" t="s">
         <v>534</v>
-      </c>
-      <c r="E2" t="s">
-        <v>578</v>
-      </c>
-      <c r="F2" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E4" t="s">
+        <v>576</v>
+      </c>
+      <c r="F4" t="s">
         <v>579</v>
-      </c>
-      <c r="F4" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E5" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B10" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B13" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B18" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -7231,16 +7228,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>529</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>530</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>531</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>532</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>94</v>
@@ -7252,45 +7249,45 @@
         <v>95</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -7336,7 +7333,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>387</v>
@@ -7386,7 +7383,7 @@
         <v>263</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>264</v>
@@ -7488,7 +7485,7 @@
         <v>293</v>
       </c>
       <c r="AK1" s="29" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AL1" s="29" t="s">
         <v>294</v>
@@ -7511,13 +7508,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>612</v>
-      </c>
       <c r="C2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7526,10 +7523,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
+        <v>612</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>613</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>614</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7617,7 +7614,7 @@
         <v>180</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AL2" s="17" t="s">
         <v>181</v>
@@ -7666,7 +7663,7 @@
         <v>295</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>296</v>
@@ -7743,10 +7740,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>630</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>631</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7850,7 +7847,7 @@
         <v>319</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>320</v>
@@ -7867,16 +7864,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>634</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>635</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7909,7 +7906,7 @@
         <v>322</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>323</v>
@@ -8064,10 +8061,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8082,16 +8079,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I2" s="20" t="s">
+        <v>617</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>618</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>619</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8115,13 +8112,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8154,10 +8151,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 28-SEP-20 part 9
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E785E-CB79-4548-977F-C12EE7D8F725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79989C8B-4F7B-4231-A117-8C69337B57A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="16" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1892,91 +1892,91 @@
     <t>12345Dummil</t>
   </si>
   <si>
-    <t>28-SEP-08-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-08-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-08-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-08-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-09-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-09-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-09-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-09-20-Drg 22.22 mEq(Enema)</t>
   </si>
 </sst>
 </file>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-08-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-09-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -6152,7 +6152,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 29-SEP-20 part 1 as 5 for jenkins demo
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79989C8B-4F7B-4231-A117-8C69337B57A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FA022-9631-437A-BFC7-18771FA2E6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="16" activeTab="17" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1877,9 +1877,6 @@
     <t>16-JUN-3-20-Pharm1-C</t>
   </si>
   <si>
-    <t>586.iu45-LT3</t>
-  </si>
-  <si>
     <t>30-Sep-2020</t>
   </si>
   <si>
@@ -1892,91 +1889,96 @@
     <t>12345Dummil</t>
   </si>
   <si>
-    <t>28-SEP-09-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-09-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-09-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-09-20-Drg 22.22 mEq(Enema)</t>
+    <t>28-SEP-12-20-PROT</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-12-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-12-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-FN</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-LN</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>28-SEP-12-20-Drg
+22.22 mEq
+(Enema)</t>
+  </si>
+  <si>
+    <t>586.iu45-LT3-U</t>
   </si>
 </sst>
 </file>
@@ -3510,10 +3512,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>610</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>611</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3522,10 +3524,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>612</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>613</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3885,7 +3887,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3900,16 +3902,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>614</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>615</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>617</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>618</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3933,13 +3935,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3972,10 +3974,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4028,7 +4030,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-09-20-Drg-Unit 22.22 mEq</v>
+        <v>28-SEP-12-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4172,7 +4174,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4275,13 +4277,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>621</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4433,13 +4435,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>623</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>624</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>625</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4451,13 +4453,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>626</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>627</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4590,10 +4592,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4887,16 +4889,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C47" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5354,13 +5356,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>624</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>625</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5372,13 +5374,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>626</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>627</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5438,8 +5440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFFB398-D4A3-48F4-A43E-4EBC96369A2B}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5525,10 +5527,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5542,10 +5544,10 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>605</v>
+        <v>638</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
@@ -5586,7 +5588,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5658,10 +5660,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5670,13 +5672,13 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>605</v>
+        <v>638</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
@@ -5714,7 +5716,7 @@
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5722,7 +5724,7 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -5863,16 +5865,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>605</v>
+        <v>638</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -6055,7 +6057,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6130,10 +6132,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -6151,8 +6153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E63512-8B54-43D1-9A38-91DAF3F128E4}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6228,16 +6230,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D2" t="s">
+        <v>607</v>
+      </c>
+      <c r="F2" t="s">
         <v>608</v>
-      </c>
-      <c r="D2" t="s">
-        <v>608</v>
-      </c>
-      <c r="F2" t="s">
-        <v>609</v>
       </c>
       <c r="G2" t="s">
         <v>514</v>
@@ -6249,16 +6251,16 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -6787,7 +6789,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6807,7 +6809,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6850,7 +6852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC81619-0CB1-4965-B466-0CE429F0B373}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6883,13 +6887,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -6919,7 +6923,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
@@ -6947,18 +6951,18 @@
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D2" s="37">
-        <v>20</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
         <v>510</v>
@@ -7508,13 +7512,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>609</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>611</v>
-      </c>
       <c r="C2" s="17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7523,10 +7527,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>612</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>613</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7740,10 +7744,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>629</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>630</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7864,16 +7868,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>631</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>633</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>634</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7889,8 +7893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C02648-616D-42A5-9175-58AAD7AE2F9C}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8061,10 +8065,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8079,16 +8083,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I2" s="20" t="s">
+        <v>616</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>617</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>618</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8103,7 +8107,7 @@
         <v>192</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>194</v>
@@ -8112,13 +8116,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8151,10 +8155,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 30-SEP-20- Par
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FA022-9631-437A-BFC7-18771FA2E6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC72F26-8744-4AA7-8F92-01B282948C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="10" activeTab="10" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="6" activeTab="6" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1889,96 +1889,96 @@
     <t>12345Dummil</t>
   </si>
   <si>
-    <t>28-SEP-12-20-PROT</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-12-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-12-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-FN</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-LN</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>28-SEP-12-20-Drg
+    <t>586.iu45-LT3-U</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PROT</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-Supplier-1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>30-SEP-01-Supplier-2</t>
+  </si>
+  <si>
+    <t>30-SEP-01-Supplier-3</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-FN</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-LN</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>30-SEP-01-20-Drg
 22.22 mEq
 (Enema)</t>
-  </si>
-  <si>
-    <t>586.iu45-LT3-U</t>
   </si>
 </sst>
 </file>
@@ -3512,10 +3512,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3524,10 +3524,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3887,7 +3887,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3902,16 +3902,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3935,13 +3935,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3974,10 +3974,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>28-SEP-12-20-Drg-Unit 22.22 mEq</v>
+        <v>30-SEP-01-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4174,7 +4174,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4277,13 +4277,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4435,13 +4435,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4453,13 +4453,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4592,10 +4592,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4889,16 +4889,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C47" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5356,13 +5356,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5374,13 +5374,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5440,7 +5440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFFB398-D4A3-48F4-A43E-4EBC96369A2B}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -5527,10 +5527,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5544,7 +5544,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>638</v>
+        <v>609</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>240</v>
@@ -5660,10 +5660,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5672,13 +5672,13 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>638</v>
+        <v>609</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
@@ -5865,16 +5865,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>609</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>622</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>636</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>638</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -6132,10 +6132,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
         <v>607</v>
@@ -6251,7 +6251,7 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="P2">
         <v>230</v>
@@ -6771,7 +6771,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6789,7 +6789,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6853,7 +6853,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6887,13 +6887,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2" t="s">
         <v>623</v>
       </c>
-      <c r="B2" t="s">
-        <v>622</v>
-      </c>
       <c r="C2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -6953,13 +6953,13 @@
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D2" s="37">
         <v>230</v>
@@ -7512,13 +7512,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7527,10 +7527,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7649,8 +7649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B189598-4DA9-43C3-A7E7-FA94EEA5CFDF}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7744,10 +7744,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7868,16 +7868,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -8065,10 +8065,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8083,16 +8083,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8116,13 +8116,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8155,10 +8155,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 30-SEP-20- Part 3
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC72F26-8744-4AA7-8F92-01B282948C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61EFF8A-5F76-4E28-815D-40F5C87F8631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="6" activeTab="6" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="4" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1892,91 +1892,91 @@
     <t>586.iu45-LT3-U</t>
   </si>
   <si>
-    <t>30-SEP-01-20-PROT</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-Supplier-1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>30-SEP-01-Supplier-2</t>
-  </si>
-  <si>
-    <t>30-SEP-01-Supplier-3</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-FN</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-LN</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>30-SEP-01-20-Drg
+    <t>30-SEP-03-20-PROT</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-Supplier-1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>30-SEP-03-Supplier-2</t>
+  </si>
+  <si>
+    <t>30-SEP-03-Supplier-3</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-FN</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-LN</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>30-SEP-03-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>30-SEP-01-20-Drg-Unit 22.22 mEq</v>
+        <v>30-SEP-03-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7305,7 +7305,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7361,8 +7361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F0EE5-7486-4F73-A47D-62B6ADC7A71D}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7649,8 +7649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B189598-4DA9-43C3-A7E7-FA94EEA5CFDF}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 01-OCT-20- Part 1-1
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61EFF8A-5F76-4E28-815D-40F5C87F8631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC00FC-1B7C-4497-AFFD-99A61544FE22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="4" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1892,91 +1892,91 @@
     <t>586.iu45-LT3-U</t>
   </si>
   <si>
-    <t>30-SEP-03-20-PROT</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-Supplier-1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>30-SEP-03-Supplier-2</t>
-  </si>
-  <si>
-    <t>30-SEP-03-Supplier-3</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-FN</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-LN</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>30-SEP-03-20-Drg
+    <t>01-OCT-20-20-PROT</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>01-OCT-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>01-OCT-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-FN</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-LN</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>01-OCT-20-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>30-SEP-03-20-Drg-Unit 22.22 mEq</v>
+        <v>01-OCT-20-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7362,7 +7362,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 1
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC00FC-1B7C-4497-AFFD-99A61544FE22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A224EA-D3C7-4C9A-8002-490504F4413B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="4" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -25,21 +25,22 @@
     <sheet name="Patient" sheetId="4" r:id="rId10"/>
     <sheet name="Receive" sheetId="5" r:id="rId11"/>
     <sheet name="TransferToPharmacy" sheetId="6" r:id="rId12"/>
-    <sheet name="Dispense" sheetId="7" r:id="rId13"/>
-    <sheet name="PatReturn" sheetId="9" r:id="rId14"/>
-    <sheet name="Destroy" sheetId="11" r:id="rId15"/>
-    <sheet name="ReturnToSupplier" sheetId="12" r:id="rId16"/>
-    <sheet name="ServiceMaster" sheetId="19" r:id="rId17"/>
-    <sheet name="CPP" sheetId="20" r:id="rId18"/>
-    <sheet name="CDM" sheetId="21" r:id="rId19"/>
-    <sheet name="Facility" sheetId="22" r:id="rId20"/>
-    <sheet name="Payer" sheetId="23" r:id="rId21"/>
-    <sheet name="ServicedEntity" sheetId="24" r:id="rId22"/>
-    <sheet name="ReviewCharges" sheetId="26" r:id="rId23"/>
-    <sheet name="ReceiveAdjust" sheetId="13" r:id="rId24"/>
-    <sheet name="TransferAdjust" sheetId="14" r:id="rId25"/>
-    <sheet name="DestroyAdjust" sheetId="15" r:id="rId26"/>
-    <sheet name="ReturnToSupplierAdjust" sheetId="16" r:id="rId27"/>
+    <sheet name="DispenseAdjust" sheetId="29" r:id="rId13"/>
+    <sheet name="Dispense" sheetId="7" r:id="rId14"/>
+    <sheet name="PatReturn" sheetId="9" r:id="rId15"/>
+    <sheet name="Destroy" sheetId="11" r:id="rId16"/>
+    <sheet name="ReturnToSupplier" sheetId="12" r:id="rId17"/>
+    <sheet name="ServiceMaster" sheetId="19" r:id="rId18"/>
+    <sheet name="CPP" sheetId="20" r:id="rId19"/>
+    <sheet name="CDM" sheetId="21" r:id="rId20"/>
+    <sheet name="Facility" sheetId="22" r:id="rId21"/>
+    <sheet name="Payer" sheetId="23" r:id="rId22"/>
+    <sheet name="ServicedEntity" sheetId="24" r:id="rId23"/>
+    <sheet name="ReviewCharges" sheetId="26" r:id="rId24"/>
+    <sheet name="ReceiveAdjust" sheetId="13" r:id="rId25"/>
+    <sheet name="TransferAdjust" sheetId="14" r:id="rId26"/>
+    <sheet name="DestroyAdjust" sheetId="15" r:id="rId27"/>
+    <sheet name="ReturnToSupplierAdjust" sheetId="16" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="642">
   <si>
     <t>UserName</t>
   </si>
@@ -1874,9 +1875,6 @@
     <t>QWAP-0101</t>
   </si>
   <si>
-    <t>16-JUN-3-20-Pharm1-C</t>
-  </si>
-  <si>
     <t>30-Sep-2020</t>
   </si>
   <si>
@@ -1889,94 +1887,106 @@
     <t>12345Dummil</t>
   </si>
   <si>
-    <t>586.iu45-LT3-U</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PROT</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>01-OCT-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>01-OCT-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-FN</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-LN</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>01-OCT-20-20-Drg
+    <t>587-LT-L</t>
+  </si>
+  <si>
+    <t>01-AUG-06-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>dispense-adjust-protocol</t>
+  </si>
+  <si>
+    <t>dispense-adjust-drug-name</t>
+  </si>
+  <si>
+    <t>dispenseadjust-esign</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-01-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-01-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-01-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -2365,7 +2375,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3512,10 +3532,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3524,10 +3544,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3887,7 +3907,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3902,16 +3922,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3935,13 +3955,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3974,10 +3994,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4030,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>01-OCT-20-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-01-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4174,7 +4194,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4277,13 +4297,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4435,13 +4455,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4453,13 +4473,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4592,10 +4612,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4889,16 +4909,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C47" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5263,7 +5283,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5356,13 +5376,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5374,13 +5394,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5441,7 +5461,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5527,10 +5547,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5544,10 +5564,10 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
@@ -5588,7 +5608,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5660,10 +5680,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5672,19 +5692,19 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>227</v>
@@ -5712,11 +5732,61 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED295A5-BB50-4478-B5AC-C5591A9D690E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>610</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>608</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:D1">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66856262-9FC7-44EB-98DF-8D229C6B1BEB}">
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5865,16 +5935,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5882,7 +5952,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>223</v>
@@ -5937,16 +6007,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:AR1">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:AR1">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA50097E-904E-4C5F-807B-5BFDC892566A}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -5978,16 +6048,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50005C1C-2D59-471B-9BB8-E0E83160DD2F}">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -6043,16 +6113,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:N1">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:N1">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A42D587-F48E-4EF1-AA1F-23324738C752}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -6099,16 +6169,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:K1">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:K1">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D3DAB8-93B0-4760-9DDD-BD773E40A52D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6132,24 +6202,24 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="B2" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E63512-8B54-43D1-9A38-91DAF3F128E4}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -6230,16 +6300,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D2" t="s">
+        <v>606</v>
+      </c>
+      <c r="F2" t="s">
         <v>607</v>
-      </c>
-      <c r="D2" t="s">
-        <v>607</v>
-      </c>
-      <c r="F2" t="s">
-        <v>608</v>
       </c>
       <c r="G2" t="s">
         <v>514</v>
@@ -6251,75 +6321,25 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 C1:T1">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{6D6C5B85-5BD9-4138-995B-87CEE9374CF9}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5B8833-1D1E-4356-A838-B98047FA7158}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6767,6 +6787,56 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5B8833-1D1E-4356-A838-B98047FA7158}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14682C1A-A86D-4C5D-B3D9-0D5F958B3EAC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6789,22 +6859,22 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="B2" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834C0E1-2ED0-48E8-8D6B-EFEED6FDF4E2}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -6839,16 +6909,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC81619-0CB1-4965-B466-0CE429F0B373}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -6887,13 +6957,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C2" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -6904,16 +6974,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFAD531-C8ED-45C2-B1A2-9642934157FA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -6953,13 +7023,13 @@
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D2" s="37">
         <v>230</v>
@@ -6973,16 +7043,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8726B607-4FF5-4DF0-BBA1-3FCDBD3D0C76}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6994,7 +7064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428AC387-3CDC-4E5F-B0D8-F4C06660CF08}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7006,7 +7076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD543CE2-8AA7-4742-B4D5-FFAFE66E2413}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7020,7 +7090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3F60D2-8704-4C3A-987D-064E20473D5E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7218,7 +7288,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7345,10 +7415,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7362,14 +7432,14 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
@@ -7512,13 +7582,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7527,10 +7597,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7744,10 +7814,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7868,16 +7938,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7893,8 +7963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C02648-616D-42A5-9175-58AAD7AE2F9C}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8065,10 +8135,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8083,16 +8153,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8107,7 +8177,7 @@
         <v>192</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>194</v>
@@ -8116,13 +8186,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8155,10 +8225,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 2
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A224EA-D3C7-4C9A-8002-490504F4413B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAE011F-3B6B-44B9-9346-83E1F1950BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-01-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-01-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-01-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-01-20-Drg
+    <t>08-OCT-02-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-02-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-02-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-02-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-01-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-02-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 2-1
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAE011F-3B6B-44B9-9346-83E1F1950BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B5BA22-4131-4C47-813B-C27941641DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 3
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B5BA22-4131-4C47-813B-C27941641DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB136933-FD6A-451D-90B5-3D5A67EFA440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-02-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-02-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-02-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-02-20-Drg
+    <t>08-OCT-03-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-03-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-03-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-03-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-02-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-03-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 4
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB136933-FD6A-451D-90B5-3D5A67EFA440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5AD8EB-A24E-4A2C-AB47-FBAC395E56B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-03-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-03-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-03-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-03-20-Drg
+    <t>08-OCT-04-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-04-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-04-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-04-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-03-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-04-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 5
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5AD8EB-A24E-4A2C-AB47-FBAC395E56B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F0D810-F29D-4FBA-ABBF-CEF48CC9632D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-04-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-04-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-04-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-04-20-Drg
+    <t>08-OCT-05-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-05-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-05-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-05-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-04-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-05-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 08-OCT-20 Part 6-1
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F0D810-F29D-4FBA-ABBF-CEF48CC9632D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E529B5C-354C-4EB2-885D-CB12C2FF2B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-05-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-05-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-05-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-05-20-Drg
+    <t>08-OCT-06-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-06-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-06-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-06-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-05-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-06-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 09-OCT-20 committing sample
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E529B5C-354C-4EB2-885D-CB12C2FF2B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87E8854-1C9E-470E-90DA-E46E30EAB9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -7432,7 +7432,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 09-OCT-20 part 7
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87E8854-1C9E-470E-90DA-E46E30EAB9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD7915-A1BE-49B4-9CA1-6403ADF725BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="4" activeTab="8" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>08-OCT-06-20-PROT</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-06-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-06-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-FN</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-LN</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>08-OCT-06-20-Drg
+    <t>08-OCT-07-20-PROT</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-07-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-07-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-FN</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-LN</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>08-OCT-07-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>08-OCT-06-20-Drg-Unit 22.22 mEq</v>
+        <v>08-OCT-07-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7431,8 +7431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F0EE5-7486-4F73-A47D-62B6ADC7A71D}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7963,8 +7963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C02648-616D-42A5-9175-58AAD7AE2F9C}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 15-OCT-20 part 2
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BE5510-2DF6-4653-AC8C-028CBA0B5B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6D7A3-07FB-44C9-9C43-AA1901F322A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1902,91 +1902,91 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>15-OCT-01-20-Drg</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PROT</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-01-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-01-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-FN</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-LN</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>15-OCT-01-20-Drg
+    <t>15-OCT-02-20-PROT</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-02-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-02-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-FN</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-LN</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>15-OCT-02-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -3532,10 +3532,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3544,10 +3544,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3907,7 +3907,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3922,16 +3922,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3955,13 +3955,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3994,10 +3994,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>15-OCT-01-20-Drg-Unit 22.22 mEq</v>
+        <v>15-OCT-02-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4194,7 +4194,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4297,13 +4297,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4455,13 +4455,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4473,13 +4473,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4612,10 +4612,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4909,16 +4909,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="C47" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5376,13 +5376,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5394,13 +5394,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5547,10 +5547,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5680,10 +5680,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5692,13 +5692,13 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>608</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
@@ -5763,7 +5763,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>640</v>
@@ -5935,10 +5935,10 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>640</v>
@@ -6202,10 +6202,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" t="s">
         <v>613</v>
-      </c>
-      <c r="B2" t="s">
-        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" t="s">
         <v>606</v>
@@ -6321,7 +6321,7 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="P2">
         <v>230</v>
@@ -6859,7 +6859,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6957,13 +6957,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="C2" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -7023,7 +7023,7 @@
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
@@ -7582,13 +7582,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7597,10 +7597,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7814,10 +7814,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7938,16 +7938,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>619</v>
+        <v>634</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>637</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>639</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7964,7 +7964,7 @@
   <dimension ref="A1:AZ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8135,10 +8135,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>614</v>
+        <v>638</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8153,16 +8153,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>616</v>
+        <v>639</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8186,13 +8186,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>619</v>
+        <v>634</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8225,10 +8225,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 15-OCT-20 part 5
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6D7A3-07FB-44C9-9C43-AA1901F322A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9B3A1-2C58-445E-BCE8-EAE140F3D60D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="643">
   <si>
     <t>UserName</t>
   </si>
@@ -1902,91 +1902,94 @@
     <t>dispenseadjust-esign</t>
   </si>
   <si>
-    <t>15-OCT-02-20-PROT</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-02-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-02-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-FN</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-LN</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>15-OCT-02-20-Drg
+    <t>01-01-2021</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PROT</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-05-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-05-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-FN</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-LN</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>15-OCT-05-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -3532,10 +3535,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3544,10 +3547,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3907,7 +3910,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3922,16 +3925,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3955,13 +3958,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -3994,10 +3997,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4050,7 +4053,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>15-OCT-02-20-Drg-Unit 22.22 mEq</v>
+        <v>15-OCT-05-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4194,7 +4197,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4297,13 +4300,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -4455,13 +4458,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4473,13 +4476,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4612,10 +4615,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4909,16 +4912,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C47" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -5376,13 +5379,13 @@
     </row>
     <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5394,13 +5397,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5547,10 +5550,10 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5680,10 +5683,10 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C2" s="23">
         <v>22.22</v>
@@ -5692,13 +5695,13 @@
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>608</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
@@ -5763,10 +5766,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>608</v>
@@ -5935,13 +5938,13 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>608</v>
@@ -6202,10 +6205,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -6300,7 +6303,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" t="s">
         <v>606</v>
@@ -6321,7 +6324,7 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P2">
         <v>230</v>
@@ -6859,7 +6862,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6957,13 +6960,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2" t="s">
         <v>627</v>
       </c>
-      <c r="B2" t="s">
-        <v>626</v>
-      </c>
       <c r="C2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -7023,13 +7026,13 @@
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D2" s="37">
         <v>230</v>
@@ -7431,8 +7434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F0EE5-7486-4F73-A47D-62B6ADC7A71D}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7582,13 +7585,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7597,10 +7600,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7640,7 +7643,7 @@
         <v>164</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>165</v>
+        <v>613</v>
       </c>
       <c r="V2" s="17" t="s">
         <v>166</v>
@@ -7814,10 +7817,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7938,16 +7941,16 @@
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7963,8 +7966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C02648-616D-42A5-9175-58AAD7AE2F9C}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8135,10 +8138,10 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
@@ -8153,16 +8156,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8186,13 +8189,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8225,10 +8228,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>

<commit_message>
committing on 15-OCT-20 part 8
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9B3A1-2C58-445E-BCE8-EAE140F3D60D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E07AC-F42B-420D-80DE-97756678B3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -1905,91 +1905,91 @@
     <t>01-01-2021</t>
   </si>
   <si>
-    <t>15-OCT-05-20-PROT</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-05-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-05-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-FN</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-LN</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>15-OCT-05-20-Drg
+    <t>15-OCT-08-20-PROT</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PROT-Title</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PROT-SPID</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PROT-SP</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-Unit</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-dl1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-id1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-adn1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Pharm1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-08-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-08-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PAT1-1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-FN</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-LN</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PAT1-STY</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PROT-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Supplier-1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Supplier-2</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Supplier-3</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-Edit</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg-DID1</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>15-OCT-08-20-Drg
 22.22 mEq
 (Enema)</t>
   </si>
@@ -4053,7 +4053,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>15-OCT-05-20-Drg-Unit 22.22 mEq</v>
+        <v>15-OCT-08-20-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -7434,8 +7434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F0EE5-7486-4F73-A47D-62B6ADC7A71D}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
committing on 15-OCT-20 part 8-C
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E07AC-F42B-420D-80DE-97756678B3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4CB76D-B5B1-444C-AE15-C9FF659D41D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="644">
   <si>
     <t>UserName</t>
   </si>
@@ -1992,6 +1992,9 @@
     <t>15-OCT-08-20-Drg
 22.22 mEq
 (Enema)</t>
+  </si>
+  <si>
+    <t>10-10-2021</t>
   </si>
 </sst>
 </file>
@@ -7435,7 +7438,7 @@
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7658,7 +7661,7 @@
         <v>169</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>170</v>
+        <v>643</v>
       </c>
       <c r="AA2" s="17" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
committing on 23-Mar-21 part 1
</commit_message>
<xml_diff>
--- a/DataProvider/Nost_Data_Driven_DP.xlsx
+++ b/DataProvider/Nost_Data_Driven_DP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jagan\NostAuto\NostCore\NostArtifact\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4CB76D-B5B1-444C-AE15-C9FF659D41D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4928ED3D-ABF0-40C5-A20E-4432DA3BEAB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="5" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="6" activeTab="12" xr2:uid="{A81F5EE2-BBD7-4667-BFC6-C75E6A3565AF}"/>
   </bookViews>
   <sheets>
     <sheet name="NostData (2)" sheetId="18" r:id="rId1"/>
@@ -25,8 +25,8 @@
     <sheet name="Patient" sheetId="4" r:id="rId10"/>
     <sheet name="Receive" sheetId="5" r:id="rId11"/>
     <sheet name="TransferToPharmacy" sheetId="6" r:id="rId12"/>
-    <sheet name="DispenseAdjust" sheetId="29" r:id="rId13"/>
-    <sheet name="Dispense" sheetId="7" r:id="rId14"/>
+    <sheet name="Dispense" sheetId="7" r:id="rId13"/>
+    <sheet name="DispenseAdjust" sheetId="29" r:id="rId14"/>
     <sheet name="PatReturn" sheetId="9" r:id="rId15"/>
     <sheet name="Destroy" sheetId="11" r:id="rId16"/>
     <sheet name="ReturnToSupplier" sheetId="12" r:id="rId17"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="645">
   <si>
     <t>UserName</t>
   </si>
@@ -1845,9 +1845,6 @@
     <t>3340354-U</t>
   </si>
   <si>
-    <t>QWAP-</t>
-  </si>
-  <si>
     <t>Drug_Name_edit</t>
   </si>
   <si>
@@ -1863,18 +1860,9 @@
     <t>6 tabs twice a day</t>
   </si>
   <si>
-    <t>Dispense 3</t>
-  </si>
-  <si>
-    <t>3rd visit</t>
-  </si>
-  <si>
     <t>aithentchn</t>
   </si>
   <si>
-    <t>QWAP-0101</t>
-  </si>
-  <si>
     <t>30-Sep-2020</t>
   </si>
   <si>
@@ -1890,9 +1878,6 @@
     <t>587-LT-L</t>
   </si>
   <si>
-    <t>01-AUG-06-20-PHARM-1-C</t>
-  </si>
-  <si>
     <t>dispense-adjust-protocol</t>
   </si>
   <si>
@@ -1905,96 +1890,114 @@
     <t>01-01-2021</t>
   </si>
   <si>
-    <t>15-OCT-08-20-PROT</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PROT-Title</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PROT-SPID</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PROT-SP</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-Unit</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-dl1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-id1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-nsc1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-adn1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Pharm1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-08-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-08-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PAT1-1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-FN</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-LN</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PAT1-STY</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PROT-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PHARM-1-C</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-PHARM-1-C-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Supplier-1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Supplier-1-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Supplier-2</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Supplier-3</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-Edit</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg-DID1</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg 22.22mEq</t>
-  </si>
-  <si>
-    <t>15-OCT-08-20-Drg
+    <t>10-10-2021</t>
+  </si>
+  <si>
+    <t>19mar21-02-U</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>QUAT-</t>
+  </si>
+  <si>
+    <t>03-AUG-03-20-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>QUAT-C</t>
+  </si>
+  <si>
+    <t>1st visit</t>
+  </si>
+  <si>
+    <t>1st Dispense</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PROT</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PROT-Title</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PROT-SPID</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PROT-SP</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-Unit</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-dl1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-id1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-nsc1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-adn1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Supplier-1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Pharm1-C</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Supplier-2</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Supplier-3</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PAT1-1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-FN</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-LN</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PAT1-STY</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PROT-Edit</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PHARM-1-C</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-PHARM-1-C-Edit</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Supplier-1-Edit</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-Edit</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg-DID1</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg 87.23mEq</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg 22.22mEq</t>
+  </si>
+  <si>
+    <t>23-Mar-21-01-Drg
 22.22 mEq
 (Enema)</t>
-  </si>
-  <si>
-    <t>10-10-2021</t>
   </si>
 </sst>
 </file>
@@ -2331,6 +2334,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2348,33 +2378,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2934,9 +2937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA99D99E-83A6-4530-A5D4-2D8973ADF18B}">
   <dimension ref="A1:CW101"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3274,16 +3277,16 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -3322,51 +3325,51 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="56" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="57"/>
-      <c r="AA7" s="58"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="49"/>
       <c r="AB7" s="50" t="s">
         <v>143</v>
       </c>
@@ -3538,10 +3541,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>152</v>
@@ -3550,10 +3553,10 @@
         <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>231</v>
@@ -3677,80 +3680,80 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="53"/>
-      <c r="Y12" s="53"/>
-      <c r="Z12" s="53"/>
-      <c r="AA12" s="53"/>
-      <c r="AB12" s="53"/>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="53"/>
-      <c r="AE12" s="53"/>
-      <c r="AF12" s="53"/>
-      <c r="AG12" s="53" t="s">
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="46"/>
+      <c r="AB12" s="46"/>
+      <c r="AC12" s="46"/>
+      <c r="AD12" s="46"/>
+      <c r="AE12" s="46"/>
+      <c r="AF12" s="46"/>
+      <c r="AG12" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="AH12" s="53"/>
-      <c r="AI12" s="53"/>
-      <c r="AJ12" s="53"/>
-      <c r="AK12" s="53"/>
-      <c r="AL12" s="53"/>
-      <c r="AM12" s="53" t="s">
+      <c r="AH12" s="46"/>
+      <c r="AI12" s="46"/>
+      <c r="AJ12" s="46"/>
+      <c r="AK12" s="46"/>
+      <c r="AL12" s="46"/>
+      <c r="AM12" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="AN12" s="53"/>
-      <c r="AO12" s="53"/>
-      <c r="AP12" s="53"/>
-      <c r="AQ12" s="53"/>
-      <c r="AR12" s="53"/>
-      <c r="AS12" s="53"/>
-      <c r="AT12" s="53"/>
-      <c r="AU12" s="53"/>
-      <c r="AV12" s="53"/>
-      <c r="AW12" s="53"/>
-      <c r="AX12" s="53"/>
-      <c r="AY12" s="53"/>
-      <c r="AZ12" s="53"/>
+      <c r="AN12" s="46"/>
+      <c r="AO12" s="46"/>
+      <c r="AP12" s="46"/>
+      <c r="AQ12" s="46"/>
+      <c r="AR12" s="46"/>
+      <c r="AS12" s="46"/>
+      <c r="AT12" s="46"/>
+      <c r="AU12" s="46"/>
+      <c r="AV12" s="46"/>
+      <c r="AW12" s="46"/>
+      <c r="AX12" s="46"/>
+      <c r="AY12" s="46"/>
+      <c r="AZ12" s="46"/>
     </row>
     <row r="13" spans="1:101" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3908,12 +3911,12 @@
       </c>
       <c r="AZ13" s="15"/>
     </row>
-    <row r="14" spans="1:101" ht="72" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:101" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>188</v>
@@ -3928,16 +3931,16 @@
         <v>190</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>191</v>
@@ -3961,13 +3964,13 @@
         <v>48</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>222</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="U14" s="17" t="s">
         <v>226</v>
@@ -4000,10 +4003,10 @@
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
       <c r="AG14" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="AH14" s="17" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="AI14" s="22"/>
       <c r="AJ14" s="22"/>
@@ -4056,7 +4059,7 @@
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B14," ",D14," ",E14)</f>
-        <v>15-OCT-08-20-Drg-Unit 22.22 mEq</v>
+        <v>23-Mar-21-01-Drg-Unit 22.22 mEq</v>
       </c>
       <c r="N15" t="s">
         <v>193</v>
@@ -4072,16 +4075,16 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -4106,16 +4109,16 @@
       <c r="N17" s="51"/>
       <c r="O17" s="51"/>
       <c r="P17" s="52"/>
-      <c r="Q17" s="53" t="s">
+      <c r="Q17" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.35">
@@ -4200,7 +4203,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>192</v>
@@ -4303,29 +4306,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="55"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -4341,48 +4344,48 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="49"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="53"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
     </row>
     <row r="28" spans="1:27" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -4461,13 +4464,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>234</v>
@@ -4479,13 +4482,13 @@
         <v>153</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
@@ -4533,16 +4536,16 @@
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="55"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
@@ -4618,10 +4621,10 @@
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -4863,16 +4866,16 @@
       <c r="A45" s="6">
         <v>35</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="49"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="58"/>
     </row>
     <row r="46" spans="1:21" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
@@ -4915,16 +4918,16 @@
         <v>37</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="C47" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>257</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>226</v>
@@ -4972,16 +4975,16 @@
       <c r="A50" s="6">
         <v>40</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="46"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="55"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
@@ -5007,16 +5010,16 @@
       <c r="A55" s="6">
         <v>45</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="46"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="54"/>
+      <c r="I55" s="55"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
@@ -5250,19 +5253,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="R7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AP7:AT7"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:AF12"/>
-    <mergeCell ref="AG12:AL12"/>
-    <mergeCell ref="AM12:AZ12"/>
-    <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="B55:I55"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="C17:P17"/>
@@ -5275,6 +5265,19 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B45:I45"/>
     <mergeCell ref="B50:I50"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AP7:AT7"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:AF12"/>
+    <mergeCell ref="AG12:AL12"/>
+    <mergeCell ref="AM12:AZ12"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V29" r:id="rId1" xr:uid="{DC7415B8-43F9-4A26-9C37-D97668AC92BE}"/>
@@ -5289,7 +5292,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5380,15 +5383,15 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>234</v>
@@ -5400,13 +5403,13 @@
         <v>153</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="J2" s="23">
         <v>22.22</v>
@@ -5473,7 +5476,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.5546875" customWidth="1"/>
   </cols>
@@ -5549,14 +5552,14 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="E2" s="23">
         <v>87.23</v>
@@ -5570,10 +5573,10 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
@@ -5583,7 +5586,7 @@
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="14">
-        <v>13.54</v>
+        <v>25.1</v>
       </c>
       <c r="R2" s="14">
         <v>250</v>
@@ -5592,13 +5595,13 @@
         <v>233</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="U2" s="14">
-        <v>99</v>
-      </c>
-      <c r="V2" s="14">
-        <v>121</v>
+        <v>613</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>611</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>612</v>
       </c>
       <c r="W2" s="22" t="s">
         <v>387</v>
@@ -5614,7 +5617,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5686,31 +5689,31 @@
     </row>
     <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="C2" s="23">
-        <v>22.22</v>
+        <v>87.23</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>227</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>227</v>
@@ -5723,7 +5726,7 @@
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
-        <v>603</v>
+        <v>615</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -5738,61 +5741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED295A5-BB50-4478-B5AC-C5591A9D690E}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>610</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>611</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>397</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>614</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>641</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>608</v>
-      </c>
-      <c r="D2" s="14"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B1:D1">
-    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66856262-9FC7-44EB-98DF-8D229C6B1BEB}">
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5803,7 +5756,7 @@
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5941,16 +5894,16 @@
     </row>
     <row r="2" spans="1:44" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -5958,7 +5911,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>223</v>
@@ -5967,18 +5920,18 @@
         <v>227</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
-        <v>600</v>
+        <v>617</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>601</v>
+        <v>616</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>603</v>
+        <v>615</v>
       </c>
       <c r="S2" s="14">
         <v>9</v>
@@ -6013,10 +5966,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:AR1">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:AR1">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED295A5-BB50-4478-B5AC-C5591A9D690E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>618</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:D1">
+    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6208,10 +6211,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="B2" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -6306,16 +6309,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B2" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D2" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="F2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="G2" t="s">
         <v>514</v>
@@ -6327,16 +6330,16 @@
         <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="P2">
         <v>230</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -6865,7 +6868,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="B2" s="14"/>
     </row>
@@ -6963,13 +6966,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="B2" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C2" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D2" t="s">
         <v>509</v>
@@ -7027,15 +7030,15 @@
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B2" t="s">
         <v>509</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D2" s="37">
         <v>230</v>
@@ -7413,7 +7416,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>387</v>
@@ -7437,8 +7440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F0EE5-7486-4F73-A47D-62B6ADC7A71D}">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7463,7 +7466,7 @@
         <v>263</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>264</v>
@@ -7588,13 +7591,13 @@
     </row>
     <row r="2" spans="1:43" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>152</v>
@@ -7603,10 +7606,10 @@
         <v>153</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>231</v>
@@ -7646,7 +7649,7 @@
         <v>164</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="V2" s="17" t="s">
         <v>166</v>
@@ -7661,7 +7664,7 @@
         <v>169</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>643</v>
+        <v>609</v>
       </c>
       <c r="AA2" s="17" t="s">
         <v>171</v>
@@ -7726,7 +7729,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7743,7 +7746,7 @@
         <v>295</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>296</v>
@@ -7815,15 +7818,15 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>192</v>
@@ -7906,7 +7909,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7927,7 +7930,7 @@
         <v>319</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>320</v>
@@ -7939,21 +7942,21 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>148</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>387</v>
@@ -7970,7 +7973,7 @@
   <dimension ref="A1:AZ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7986,7 +7989,7 @@
         <v>322</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>323</v>
@@ -8141,16 +8144,16 @@
     </row>
     <row r="2" spans="1:52" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>188</v>
       </c>
       <c r="D2" s="23">
-        <v>22.22</v>
+        <v>87.23</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>189</v>
@@ -8159,16 +8162,16 @@
         <v>190</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>191</v>
@@ -8183,7 +8186,7 @@
         <v>192</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>194</v>
@@ -8192,13 +8195,13 @@
         <v>48</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>223</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>227</v>
@@ -8231,10 +8234,10 @@
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="17" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="AI2" s="22"/>
       <c r="AJ2" s="22"/>

</xml_diff>